<commit_message>
fading of blob platform aand other files added. Many additions done and bug fixes
</commit_message>
<xml_diff>
--- a/Assets/Levels/testLevel.xlsx
+++ b/Assets/Levels/testLevel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar\Desktop\Level Editor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar\Documents\Eferaga\EFERAGAPC\D\Edgar\Proyectos\UnityProjects\MobileGames\Fall2015\LonelyBlob\Assets\Levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Tiles_X</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>MapData</t>
+  </si>
+  <si>
+    <t>Tile size</t>
   </si>
 </sst>
 </file>
@@ -116,305 +119,641 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
+  <dxfs count="108">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -853,31 +1192,38 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="5" customWidth="1"/>
+    <col min="6" max="7" width="4.85546875" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" customWidth="1"/>
+    <col min="10" max="10" width="4" customWidth="1"/>
+    <col min="11" max="11" width="3.85546875" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <f>COUNTA(A8:AU8)</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -889,29 +1235,35 @@
       <c r="D2" s="4"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -933,36 +1285,66 @@
       <c r="G8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -977,15 +1359,30 @@
         <v>4</v>
       </c>
       <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -1000,15 +1397,30 @@
         <v>4</v>
       </c>
       <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -1023,15 +1435,30 @@
         <v>4</v>
       </c>
       <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -1046,15 +1473,30 @@
         <v>4</v>
       </c>
       <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -1069,15 +1511,30 @@
         <v>4</v>
       </c>
       <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -1092,15 +1549,30 @@
         <v>4</v>
       </c>
       <c r="G15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -1115,15 +1587,30 @@
         <v>4</v>
       </c>
       <c r="G16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1138,15 +1625,30 @@
         <v>4</v>
       </c>
       <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -1161,15 +1663,30 @@
         <v>4</v>
       </c>
       <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -1184,15 +1701,30 @@
         <v>4</v>
       </c>
       <c r="G19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -1207,15 +1739,30 @@
         <v>4</v>
       </c>
       <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -1230,15 +1777,30 @@
         <v>4</v>
       </c>
       <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <v>4</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -1253,15 +1815,30 @@
         <v>4</v>
       </c>
       <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -1276,15 +1853,30 @@
         <v>4</v>
       </c>
       <c r="G23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -1299,15 +1891,30 @@
         <v>4</v>
       </c>
       <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -1322,15 +1929,30 @@
         <v>4</v>
       </c>
       <c r="G25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <v>4</v>
@@ -1345,15 +1967,30 @@
         <v>4</v>
       </c>
       <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>4</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -1368,15 +2005,30 @@
         <v>4</v>
       </c>
       <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>4</v>
@@ -1391,15 +2043,30 @@
         <v>4</v>
       </c>
       <c r="G28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
+      <c r="I28">
+        <v>4</v>
+      </c>
+      <c r="J28">
+        <v>4</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C29">
         <v>4</v>
@@ -1414,15 +2081,30 @@
         <v>4</v>
       </c>
       <c r="G29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <v>4</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -1437,15 +2119,30 @@
         <v>4</v>
       </c>
       <c r="G30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>4</v>
+      </c>
+      <c r="J30">
+        <v>4</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C31" s="6">
         <v>2</v>
@@ -1460,15 +2157,30 @@
         <v>4</v>
       </c>
       <c r="G31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>4</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C32">
         <v>4</v>
@@ -1483,15 +2195,30 @@
         <v>4</v>
       </c>
       <c r="G32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>4</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -1506,15 +2233,30 @@
         <v>4</v>
       </c>
       <c r="G33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H33">
+        <v>4</v>
+      </c>
+      <c r="I33">
+        <v>4</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -1529,33 +2271,63 @@
         <v>4</v>
       </c>
       <c r="G34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <v>4</v>
+      </c>
+      <c r="J34">
+        <v>4</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1577,32 +2349,201 @@
       <c r="G36">
         <v>1</v>
       </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A37:BU392 G1:BU5 C2:E2 A4:E5 B3:E3 A1:A2 D1 B1 A6:BU7 E29 B29:D30 F29:F31 B31:B35 C32:F35 D31:E31 B9:F28 A9:A36 B36:BU36 G8:BU35 A8:F8">
-    <cfRule type="expression" dxfId="44" priority="4" stopIfTrue="1">
+  <conditionalFormatting sqref="A37:BU392 G1:BU5 C2:E2 A4:E5 B3:E3 A1:A2 D1 B1 E29 C29:D30 F29:F31 D31:E31 C10:F28 C32:F34 A6:BU7 A10:A34 L10:BU34 M9:BU9 A8 C8:J8 L8:BU8 C36:F36 M35:BU36 A36">
+    <cfRule type="expression" dxfId="92" priority="52" stopIfTrue="1">
       <formula>A1=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="53" stopIfTrue="1">
       <formula>A1=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="56" stopIfTrue="1">
       <formula>A1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="42" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="49" stopIfTrue="1">
       <formula>B2="PLATF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="50" stopIfTrue="1">
       <formula>B2="ENEMY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="51" stopIfTrue="1">
       <formula>B2="BLOCK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10:J15">
+    <cfRule type="expression" dxfId="86" priority="46" stopIfTrue="1">
+      <formula>G10=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="47" stopIfTrue="1">
+      <formula>G10=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="48" stopIfTrue="1">
+      <formula>G10=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16:J22">
+    <cfRule type="expression" dxfId="83" priority="43" stopIfTrue="1">
+      <formula>G16=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="44" stopIfTrue="1">
+      <formula>G16=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="45" stopIfTrue="1">
+      <formula>G16=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23:J29">
+    <cfRule type="expression" dxfId="80" priority="40" stopIfTrue="1">
+      <formula>G23=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="79" priority="41" stopIfTrue="1">
+      <formula>G23=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="78" priority="42" stopIfTrue="1">
+      <formula>G23=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G30:J34">
+    <cfRule type="expression" dxfId="77" priority="37" stopIfTrue="1">
+      <formula>G30=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="38" stopIfTrue="1">
+      <formula>G30=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="75" priority="39" stopIfTrue="1">
+      <formula>G30=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36:J36">
+    <cfRule type="expression" dxfId="74" priority="34" stopIfTrue="1">
+      <formula>G36=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="35" stopIfTrue="1">
+      <formula>G36=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="36" stopIfTrue="1">
+      <formula>G36=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L36">
+    <cfRule type="expression" dxfId="65" priority="31" stopIfTrue="1">
+      <formula>L36=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="32" stopIfTrue="1">
+      <formula>L36=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="63" priority="33" stopIfTrue="1">
+      <formula>L36=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9 C9:J9 L9">
+    <cfRule type="expression" dxfId="59" priority="28" stopIfTrue="1">
+      <formula>A9=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="29" stopIfTrue="1">
+      <formula>A9=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="30" stopIfTrue="1">
+      <formula>A9=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:B34 B8 B36">
+    <cfRule type="expression" dxfId="53" priority="25" stopIfTrue="1">
+      <formula>B8=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="26" stopIfTrue="1">
+      <formula>B8=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="27" stopIfTrue="1">
+      <formula>B8=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" dxfId="47" priority="22" stopIfTrue="1">
+      <formula>B9=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="23" stopIfTrue="1">
+      <formula>B9=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="24" stopIfTrue="1">
+      <formula>B9=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10:K34 K8 K36">
+    <cfRule type="expression" dxfId="41" priority="19" stopIfTrue="1">
+      <formula>K8=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="20" stopIfTrue="1">
+      <formula>K8=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="21" stopIfTrue="1">
+      <formula>K8=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="expression" dxfId="35" priority="16" stopIfTrue="1">
+      <formula>K9=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="17" stopIfTrue="1">
+      <formula>K9=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="18" stopIfTrue="1">
+      <formula>K9=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35 C35:J35 L35">
+    <cfRule type="expression" dxfId="17" priority="7" stopIfTrue="1">
+      <formula>A35=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="8" stopIfTrue="1">
+      <formula>A35=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="9" stopIfTrue="1">
+      <formula>A35=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
+      <formula>B35=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="5" stopIfTrue="1">
+      <formula>B35=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
+      <formula>B35=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K35">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+      <formula>K35=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+      <formula>K35=3</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+      <formula>K35=1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A37:G39 H8:L39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A37:L39">
       <formula1>MapElem</formula1>
     </dataValidation>
   </dataValidations>
@@ -1615,7 +2556,7 @@
           <x14:formula1>
             <xm:f>Definitions!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A8:G36</xm:sqref>
+          <xm:sqref>A8:L36</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1631,7 +2572,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
@@ -1672,13 +2613,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A2 A4:A5">
-    <cfRule type="expression" dxfId="59" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="4" stopIfTrue="1">
       <formula>A1="PLATF"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="5" stopIfTrue="1">
       <formula>A1="ENEMY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="6" stopIfTrue="1">
       <formula>A1="BLOCK"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>